<commit_message>
Updated population margins to account for only sbv residents over 18 years old in population weights
</commit_message>
<xml_diff>
--- a/data/population_margins.xlsx
+++ b/data/population_margins.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janelle/Documents/2022/Ocean Rainforest/KelpWanted-Survey-Data-Analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janelle/Documents/2022/Ocean Rainforest/Kelp_Wanted_Survey_Analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{540F8042-1156-5140-B559-9B1B88282207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2074FF94-792C-344F-818C-FBD980B6DAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14800" xr2:uid="{00EEFE30-DEBC-674B-A57D-5C67A795FCA2}"/>
+    <workbookView xWindow="-30260" yWindow="-1100" windowWidth="29720" windowHeight="20600" xr2:uid="{00EEFE30-DEBC-674B-A57D-5C67A795FCA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="21">
   <si>
     <t>Age Group</t>
   </si>
@@ -46,15 +46,6 @@
     <t>Proportion of total Ventura and Santa Barbara County Residents (ACS 2019)</t>
   </si>
   <si>
-    <t>Under 5 years</t>
-  </si>
-  <si>
-    <t>5 to 9 years</t>
-  </si>
-  <si>
-    <t>10 to 14 years</t>
-  </si>
-  <si>
     <t>15 to 19 years</t>
   </si>
   <si>
@@ -94,12 +85,6 @@
     <t>75 to 79 years</t>
   </si>
   <si>
-    <t>80 to 84 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85 and over </t>
-  </si>
-  <si>
     <t>female</t>
   </si>
   <si>
@@ -110,6 +95,9 @@
   </si>
   <si>
     <t>Total Number</t>
+  </si>
+  <si>
+    <t>80 +</t>
   </si>
 </sst>
 </file>
@@ -117,7 +105,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -153,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A900F426-A9F4-E74D-BB0E-26C0A6CA9AD4}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,7 +467,7 @@
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,13 +475,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -501,17 +489,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C2">
-        <v>36406</v>
+        <f>48510*(1/5)</f>
+        <v>9702</v>
       </c>
       <c r="D2" s="2">
         <f>C2/$H$2</f>
-        <v>2.8167009025110153E-2</v>
+        <v>9.9270014439274828E-3</v>
       </c>
       <c r="H2">
-        <v>1292505</v>
+        <f>481777.4+495557</f>
+        <v>977334.4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -519,14 +509,14 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>34419</v>
+        <v>49829</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D37" si="0">C3/$H$2</f>
-        <v>2.6629684217856022E-2</v>
+        <f t="shared" ref="D3:D29" si="0">C3/$H$2</f>
+        <v>5.0984596469744646E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -534,14 +524,14 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>45524</v>
+        <v>44444</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>3.5221527189449944E-2</v>
+        <v>4.5474711623779945E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -549,14 +539,14 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>48510</v>
+        <v>38862</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>3.753176970301856E-2</v>
+        <v>3.9763258102856094E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -564,14 +554,14 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>49829</v>
+        <v>37618</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>3.8552268656600941E-2</v>
+        <v>3.8490408196007422E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -579,14 +569,14 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>44444</v>
+        <v>39026</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>3.4385940479920774E-2</v>
+        <v>3.9931061466781478E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -594,14 +584,14 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>38862</v>
+        <v>39220</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>3.0067195097891304E-2</v>
+        <v>4.0129560568010293E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -609,14 +599,14 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>37618</v>
+        <v>39659</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>2.9104722999137335E-2</v>
+        <v>4.0578741523883737E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -624,14 +614,14 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>39026</v>
+        <v>42425</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>3.0194080487116103E-2</v>
+        <v>4.3408888503259475E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -639,14 +629,14 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>39220</v>
+        <v>40867</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>3.0344176618272271E-2</v>
+        <v>4.18147565459683E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -654,14 +644,14 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>39659</v>
+        <v>33498</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>3.0683827141867924E-2</v>
+        <v>3.4274860273003797E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -669,14 +659,14 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C13">
-        <v>42425</v>
+        <v>28663</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>3.2823857547939851E-2</v>
+        <v>2.9327730610935212E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -684,360 +674,246 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>40867</v>
+        <v>18795</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>3.1618446350304252E-2</v>
+        <v>1.9230879420595447E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>33498</v>
+        <f>13702+19247</f>
+        <v>32949</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>2.5917114440563091E-2</v>
+        <v>3.3713128280351126E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>28663</v>
+        <f>47562*(1/5)</f>
+        <v>9512.4</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>2.2176316532624633E-2</v>
+        <v>9.73300438416984E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C17">
-        <v>18795</v>
+        <v>52703</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>1.4541529820000697E-2</v>
+        <v>5.3925248103412711E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C18">
-        <v>13702</v>
+        <v>46176</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>1.0601119531452489E-2</v>
+        <v>4.7246878857430986E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>19247</v>
+        <v>43673</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>1.4891238331766608E-2</v>
+        <v>4.4685831175081937E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C20">
-        <v>38355</v>
+        <v>39211</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>2.9674933559251222E-2</v>
+        <v>4.0120351846819266E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C21">
-        <v>37598</v>
+        <v>39665</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>2.908924917118309E-2</v>
+        <v>4.0584880671344421E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C22">
-        <v>46011</v>
+        <v>38286</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>3.5598314900135784E-2</v>
+        <v>3.9173899946630342E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C23">
-        <v>47562</v>
+        <v>40016</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>3.6798310257987396E-2</v>
+        <v>4.0944020797794488E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C24">
-        <v>52703</v>
+        <v>42179</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>4.0775857733625791E-2</v>
+        <v>4.3157183457371399E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C25">
-        <v>46176</v>
+        <v>37308</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>3.5725973980758295E-2</v>
+        <v>3.8173218910538702E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>43673</v>
+        <v>28370</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>3.378942441228467E-2</v>
+        <v>2.9027935576605098E-2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C27">
-        <v>39211</v>
+        <v>26908</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>3.0337213395692859E-2</v>
+        <v>2.7532029978684879E-2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>39665</v>
+        <v>16073</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>3.0688469290254195E-2</v>
+        <v>1.64457528559314E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C29">
-        <v>38286</v>
+        <f>11073+10624</f>
+        <v>21697</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>2.9621548852809081E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30">
-        <v>40016</v>
-      </c>
-      <c r="D30" s="2">
-        <f t="shared" si="0"/>
-        <v>3.0960034970851178E-2</v>
+        <v>2.2200180409080044E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31">
-        <v>42179</v>
-      </c>
-      <c r="D31" s="2">
-        <f t="shared" si="0"/>
-        <v>3.2633529464102654E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32">
-        <v>37308</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" si="0"/>
-        <v>2.8864878665846555E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33">
-        <v>28370</v>
-      </c>
-      <c r="D33" s="2">
-        <f t="shared" si="0"/>
-        <v>2.1949624953094958E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34">
-        <v>26908</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="0"/>
-        <v>2.0818488129639729E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35">
-        <v>16073</v>
-      </c>
-      <c r="D35" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2435541835428103E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36">
-        <v>11073</v>
-      </c>
-      <c r="D36" s="2">
-        <f t="shared" si="0"/>
-        <v>8.5670848468671294E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37">
-        <v>10624</v>
-      </c>
-      <c r="D37" s="2">
-        <f t="shared" si="0"/>
-        <v>8.2196974092943551E-3</v>
-      </c>
+      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>